<commit_message>
update example data connectivity
</commit_message>
<xml_diff>
--- a/braph2genesis/pipelines/connectivity-functional multiplex/example data CON-FUN_MP/xls/connectivity/GroupName2/covariates/GroupName2_covariates.xlsx
+++ b/braph2genesis/pipelines/connectivity-functional multiplex/example data CON-FUN_MP/xls/connectivity/GroupName2/covariates/GroupName2_covariates.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A745CDA-C917-4B9F-B293-D6DC79A6F86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna.canal.garcia/Documents/GitHub/Braph-2.0-Matlab/braph2genesis/pipelines/connectivity-functional multiplex/example data CON-FUN_MP/xls/connectivity/GroupName2/covariates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4472F409-4E08-DC41-8EA7-307B68D1D913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16260" yWindow="8340" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,32 +42,32 @@
     <t>sex</t>
   </si>
   <si>
-    <t>ID1</t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
-    <t>ID2</t>
-  </si>
-  <si>
-    <t>ID3</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
-    <t>ID4</t>
-  </si>
-  <si>
-    <t>ID5</t>
+    <t>ID6</t>
+  </si>
+  <si>
+    <t>ID7</t>
+  </si>
+  <si>
+    <t>ID8</t>
+  </si>
+  <si>
+    <t>ID9</t>
+  </si>
+  <si>
+    <t>ID10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,15 +432,15 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -446,40 +451,40 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>90</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -487,10 +492,10 @@
         <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -498,7 +503,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>